<commit_message>
Update example to match readme
</commit_message>
<xml_diff>
--- a/src/data/work_tasks.xlsx
+++ b/src/data/work_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luchian\OneDrive - e-uvt.ro\Year 1 Sem 1\OR\Project\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F2D4F2-D64D-4251-9243-6A6CA972F2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AA74EB-A20A-4B47-97E7-50886854EF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +480,7 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -494,7 +494,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>5</v>

</xml_diff>

<commit_message>
Add max tasks per day, change from Continuous to Integer
</commit_message>
<xml_diff>
--- a/src/data/work_tasks.xlsx
+++ b/src/data/work_tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luchian\OneDrive - e-uvt.ro\Year 1 Sem 1\OR\Project\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AA74EB-A20A-4B47-97E7-50886854EF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A8A6D4-2D82-49D8-935C-3FA8A5E18DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,7 +438,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -497,7 +497,7 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>